<commit_message>
added sales report for lots
</commit_message>
<xml_diff>
--- a/client/static/reports/lot_list/SALES_2016-04-05.xlsx
+++ b/client/static/reports/lot_list/SALES_2016-04-05.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>BENEVOLA MEMORIAL GARDEN</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>man, bat</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>P         3,060,000.00</t>
   </si>
 </sst>
 </file>
@@ -68,7 +74,7 @@
   <numFmts count="1">
     <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -90,6 +96,18 @@
       <color rgb="00000000"/>
       <sz val="11"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="12"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -99,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -114,11 +132,18 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -128,6 +153,13 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -426,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F12"/>
+  <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,7 +502,7 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
@@ -485,7 +517,7 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
@@ -500,7 +532,7 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F9" t="s">
@@ -515,7 +547,7 @@
       <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F10" t="s">
@@ -533,7 +565,7 @@
       <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F11" t="s">
@@ -551,11 +583,22 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s"/>
+      <c r="B13" t="s"/>
+      <c r="C13" t="s"/>
+      <c r="D13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>